<commit_message>
CIERRE 27 SEP 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/I R A N A   2023.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/I R A N A   2023.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="11">
   <si>
     <t xml:space="preserve">GASTOS DE  AGUA   SENDEROS        I R A N A </t>
   </si>
@@ -571,7 +571,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1065,12 +1065,18 @@
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B37" s="2"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="6"/>
+      <c r="B37" s="2">
+        <v>45195</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="6">
+        <v>-212</v>
+      </c>
       <c r="E37" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.3">
@@ -1079,7 +1085,7 @@
       <c r="D38" s="6"/>
       <c r="E38" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.3">
@@ -1088,7 +1094,7 @@
       <c r="D39" s="6"/>
       <c r="E39" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.3">
@@ -1097,7 +1103,7 @@
       <c r="D40" s="6"/>
       <c r="E40" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.3">
@@ -1106,7 +1112,7 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.3">
@@ -1115,7 +1121,7 @@
       <c r="D42" s="6"/>
       <c r="E42" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.3">
@@ -1124,7 +1130,7 @@
       <c r="D43" s="6"/>
       <c r="E43" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.3">
@@ -1133,7 +1139,7 @@
       <c r="D44" s="6"/>
       <c r="E44" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.3">
@@ -1142,7 +1148,7 @@
       <c r="D45" s="6"/>
       <c r="E45" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.3">
@@ -1151,7 +1157,7 @@
       <c r="D46" s="6"/>
       <c r="E46" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.3">
@@ -1160,7 +1166,7 @@
       <c r="D47" s="6"/>
       <c r="E47" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.3">
@@ -1169,7 +1175,7 @@
       <c r="D48" s="6"/>
       <c r="E48" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.3">
@@ -1178,7 +1184,7 @@
       <c r="D49" s="6"/>
       <c r="E49" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.3">
@@ -1187,7 +1193,7 @@
       <c r="D50" s="6"/>
       <c r="E50" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.3">
@@ -1196,7 +1202,7 @@
       <c r="D51" s="6"/>
       <c r="E51" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.3">
@@ -1205,7 +1211,7 @@
       <c r="D52" s="6"/>
       <c r="E52" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.3">
@@ -1214,7 +1220,7 @@
       <c r="D53" s="6"/>
       <c r="E53" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.3">
@@ -1223,7 +1229,7 @@
       <c r="D54" s="6"/>
       <c r="E54" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.3">
@@ -1232,7 +1238,7 @@
       <c r="D55" s="6"/>
       <c r="E55" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.3">
@@ -1241,7 +1247,7 @@
       <c r="D56" s="6"/>
       <c r="E56" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.3">
@@ -1250,7 +1256,7 @@
       <c r="D57" s="6"/>
       <c r="E57" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.3">
@@ -1259,7 +1265,7 @@
       <c r="D58" s="6"/>
       <c r="E58" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.3">
@@ -1268,7 +1274,7 @@
       <c r="D59" s="6"/>
       <c r="E59" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.3">
@@ -1277,7 +1283,7 @@
       <c r="D60" s="6"/>
       <c r="E60" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.3">
@@ -1286,7 +1292,7 @@
       <c r="D61" s="6"/>
       <c r="E61" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.3">
@@ -1295,7 +1301,7 @@
       <c r="D62" s="6"/>
       <c r="E62" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.3">
@@ -1304,7 +1310,7 @@
       <c r="D63" s="6"/>
       <c r="E63" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.3">
@@ -1313,7 +1319,7 @@
       <c r="D64" s="6"/>
       <c r="E64" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.3">
@@ -1322,7 +1328,7 @@
       <c r="D65" s="6"/>
       <c r="E65" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.3">
@@ -1331,7 +1337,7 @@
       <c r="D66" s="6"/>
       <c r="E66" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.3">
@@ -1340,7 +1346,7 @@
       <c r="D67" s="6"/>
       <c r="E67" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.3">
@@ -1349,7 +1355,7 @@
       <c r="D68" s="6"/>
       <c r="E68" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.3">
@@ -1358,7 +1364,7 @@
       <c r="D69" s="6"/>
       <c r="E69" s="6">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>122</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
cierre 30 NOV 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/I R A N A   2023.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/I R A N A   2023.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="12">
   <si>
     <t xml:space="preserve">GASTOS DE  AGUA   SENDEROS        I R A N A </t>
   </si>
@@ -593,7 +593,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D59" sqref="D59"/>
+      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1417,21 +1417,33 @@
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B59" s="2"/>
-      <c r="C59" s="19"/>
-      <c r="D59" s="6"/>
+      <c r="B59" s="2">
+        <v>45254</v>
+      </c>
+      <c r="C59" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" s="6">
+        <v>-212</v>
+      </c>
       <c r="E59" s="6">
         <f t="shared" si="0"/>
-        <v>154</v>
+        <v>-58</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B60" s="2"/>
-      <c r="C60" s="19"/>
-      <c r="D60" s="6"/>
+      <c r="B60" s="2">
+        <v>45258</v>
+      </c>
+      <c r="C60" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" s="6">
+        <v>-159</v>
+      </c>
       <c r="E60" s="6">
         <f t="shared" si="0"/>
-        <v>154</v>
+        <v>-217</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.3">
@@ -1440,7 +1452,7 @@
       <c r="D61" s="6"/>
       <c r="E61" s="6">
         <f t="shared" si="0"/>
-        <v>154</v>
+        <v>-217</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.3">
@@ -1449,7 +1461,7 @@
       <c r="D62" s="6"/>
       <c r="E62" s="6">
         <f t="shared" si="0"/>
-        <v>154</v>
+        <v>-217</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.3">
@@ -1458,7 +1470,7 @@
       <c r="D63" s="6"/>
       <c r="E63" s="6">
         <f t="shared" si="0"/>
-        <v>154</v>
+        <v>-217</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.3">
@@ -1467,7 +1479,7 @@
       <c r="D64" s="6"/>
       <c r="E64" s="6">
         <f t="shared" si="0"/>
-        <v>154</v>
+        <v>-217</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.3">
@@ -1476,7 +1488,7 @@
       <c r="D65" s="6"/>
       <c r="E65" s="6">
         <f t="shared" si="0"/>
-        <v>154</v>
+        <v>-217</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.3">
@@ -1485,7 +1497,7 @@
       <c r="D66" s="6"/>
       <c r="E66" s="6">
         <f t="shared" si="0"/>
-        <v>154</v>
+        <v>-217</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.3">
@@ -1494,7 +1506,7 @@
       <c r="D67" s="6"/>
       <c r="E67" s="6">
         <f t="shared" si="0"/>
-        <v>154</v>
+        <v>-217</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.3">
@@ -1503,7 +1515,7 @@
       <c r="D68" s="6"/>
       <c r="E68" s="6">
         <f t="shared" si="0"/>
-        <v>154</v>
+        <v>-217</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.3">
@@ -1512,7 +1524,7 @@
       <c r="D69" s="6"/>
       <c r="E69" s="6">
         <f t="shared" si="0"/>
-        <v>154</v>
+        <v>-217</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
cierre 5 DIC 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/I R A N A   2023.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/I R A N A   2023.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="12">
   <si>
     <t xml:space="preserve">GASTOS DE  AGUA   SENDEROS        I R A N A </t>
   </si>
@@ -593,7 +593,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
+      <selection pane="bottomLeft" activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1447,12 +1447,18 @@
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B61" s="2"/>
-      <c r="C61" s="19"/>
-      <c r="D61" s="6"/>
+      <c r="B61" s="2">
+        <v>45261</v>
+      </c>
+      <c r="C61" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="6">
+        <v>500</v>
+      </c>
       <c r="E61" s="6">
         <f t="shared" si="0"/>
-        <v>-217</v>
+        <v>283</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.3">
@@ -1461,7 +1467,7 @@
       <c r="D62" s="6"/>
       <c r="E62" s="6">
         <f t="shared" si="0"/>
-        <v>-217</v>
+        <v>283</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.3">
@@ -1470,7 +1476,7 @@
       <c r="D63" s="6"/>
       <c r="E63" s="6">
         <f t="shared" si="0"/>
-        <v>-217</v>
+        <v>283</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.3">
@@ -1479,7 +1485,7 @@
       <c r="D64" s="6"/>
       <c r="E64" s="6">
         <f t="shared" si="0"/>
-        <v>-217</v>
+        <v>283</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.3">
@@ -1488,7 +1494,7 @@
       <c r="D65" s="6"/>
       <c r="E65" s="6">
         <f t="shared" si="0"/>
-        <v>-217</v>
+        <v>283</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.3">
@@ -1497,7 +1503,7 @@
       <c r="D66" s="6"/>
       <c r="E66" s="6">
         <f t="shared" si="0"/>
-        <v>-217</v>
+        <v>283</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.3">
@@ -1506,7 +1512,7 @@
       <c r="D67" s="6"/>
       <c r="E67" s="6">
         <f t="shared" si="0"/>
-        <v>-217</v>
+        <v>283</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.3">
@@ -1515,7 +1521,7 @@
       <c r="D68" s="6"/>
       <c r="E68" s="6">
         <f t="shared" si="0"/>
-        <v>-217</v>
+        <v>283</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.3">
@@ -1524,7 +1530,7 @@
       <c r="D69" s="6"/>
       <c r="E69" s="6">
         <f t="shared" si="0"/>
-        <v>-217</v>
+        <v>283</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
CIERRE 12- DIC 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/I R A N A   2023.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/I R A N A   2023.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="12">
   <si>
     <t xml:space="preserve">GASTOS DE  AGUA   SENDEROS        I R A N A </t>
   </si>
@@ -592,8 +592,8 @@
   <dimension ref="B3:E70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D62" sqref="D62"/>
+      <pane ySplit="5" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1462,39 +1462,63 @@
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B62" s="2"/>
-      <c r="C62" s="19"/>
-      <c r="D62" s="6"/>
+      <c r="B62" s="2">
+        <v>45272</v>
+      </c>
+      <c r="C62" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" s="6">
+        <v>500</v>
+      </c>
       <c r="E62" s="6">
         <f t="shared" si="0"/>
-        <v>283</v>
+        <v>783</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B63" s="2"/>
-      <c r="C63" s="19"/>
-      <c r="D63" s="6"/>
+      <c r="B63" s="2">
+        <v>45261</v>
+      </c>
+      <c r="C63" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" s="6">
+        <v>-212</v>
+      </c>
       <c r="E63" s="6">
         <f t="shared" si="0"/>
-        <v>283</v>
+        <v>571</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B64" s="2"/>
-      <c r="C64" s="19"/>
-      <c r="D64" s="6"/>
+      <c r="B64" s="2">
+        <v>45265</v>
+      </c>
+      <c r="C64" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" s="6">
+        <v>-106</v>
+      </c>
       <c r="E64" s="6">
         <f t="shared" si="0"/>
-        <v>283</v>
+        <v>465</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B65" s="2"/>
-      <c r="C65" s="19"/>
-      <c r="D65" s="6"/>
+      <c r="B65" s="2">
+        <v>45268</v>
+      </c>
+      <c r="C65" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" s="6">
+        <v>-159</v>
+      </c>
       <c r="E65" s="6">
         <f t="shared" si="0"/>
-        <v>283</v>
+        <v>306</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.3">
@@ -1503,7 +1527,7 @@
       <c r="D66" s="6"/>
       <c r="E66" s="6">
         <f t="shared" si="0"/>
-        <v>283</v>
+        <v>306</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.3">
@@ -1512,7 +1536,7 @@
       <c r="D67" s="6"/>
       <c r="E67" s="6">
         <f t="shared" si="0"/>
-        <v>283</v>
+        <v>306</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.3">
@@ -1521,7 +1545,7 @@
       <c r="D68" s="6"/>
       <c r="E68" s="6">
         <f t="shared" si="0"/>
-        <v>283</v>
+        <v>306</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.3">
@@ -1530,7 +1554,7 @@
       <c r="D69" s="6"/>
       <c r="E69" s="6">
         <f t="shared" si="0"/>
-        <v>283</v>
+        <v>306</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
CIERRE 20 DIC 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/I R A N A   2023.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/I R A N A   2023.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="12">
   <si>
     <t xml:space="preserve">GASTOS DE  AGUA   SENDEROS        I R A N A </t>
   </si>
@@ -589,11 +589,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E70"/>
+  <dimension ref="B3:E83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D69" sqref="D69"/>
+      <pane ySplit="5" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -692,7 +692,7 @@
         <v>-260</v>
       </c>
       <c r="E10" s="6">
-        <f t="shared" ref="E10:E69" si="0">E9+D10</f>
+        <f t="shared" ref="E10:E73" si="0">E9+D10</f>
         <v>324</v>
       </c>
     </row>
@@ -1567,19 +1567,148 @@
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B69" s="2"/>
-      <c r="C69" s="19"/>
-      <c r="D69" s="6"/>
+      <c r="B69" s="2">
+        <v>45279</v>
+      </c>
+      <c r="C69" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D69" s="6">
+        <v>-318</v>
+      </c>
       <c r="E69" s="6">
         <f t="shared" si="0"/>
-        <v>382</v>
+        <v>64</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B70" s="2"/>
-      <c r="C70" s="19"/>
-      <c r="D70" s="6"/>
-      <c r="E70" s="6"/>
+      <c r="B70" s="2">
+        <v>45280</v>
+      </c>
+      <c r="C70" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" s="6">
+        <v>500</v>
+      </c>
+      <c r="E70" s="6">
+        <f t="shared" si="0"/>
+        <v>564</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B71" s="2"/>
+      <c r="C71" s="19"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6">
+        <f t="shared" si="0"/>
+        <v>564</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B72" s="2"/>
+      <c r="C72" s="19"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6">
+        <f t="shared" si="0"/>
+        <v>564</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B73" s="2"/>
+      <c r="C73" s="19"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6">
+        <f t="shared" si="0"/>
+        <v>564</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B74" s="2"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6">
+        <f t="shared" ref="E74:E82" si="1">E73+D74</f>
+        <v>564</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B75" s="2"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6">
+        <f t="shared" si="1"/>
+        <v>564</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B76" s="2"/>
+      <c r="C76" s="19"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6">
+        <f t="shared" si="1"/>
+        <v>564</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B77" s="2"/>
+      <c r="C77" s="19"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6">
+        <f t="shared" si="1"/>
+        <v>564</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B78" s="2"/>
+      <c r="C78" s="19"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6">
+        <f t="shared" si="1"/>
+        <v>564</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B79" s="2"/>
+      <c r="C79" s="19"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6">
+        <f t="shared" si="1"/>
+        <v>564</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B80" s="2"/>
+      <c r="C80" s="19"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6">
+        <f t="shared" si="1"/>
+        <v>564</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B81" s="2"/>
+      <c r="C81" s="19"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6">
+        <f t="shared" si="1"/>
+        <v>564</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B82" s="2"/>
+      <c r="C82" s="19"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6">
+        <f t="shared" si="1"/>
+        <v>564</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B83" s="2"/>
+      <c r="C83" s="19"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>